<commit_message>
Finished Mastery Topic Slides 6 and 7
</commit_message>
<xml_diff>
--- a/MAP.xlsx
+++ b/MAP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
   <si>
     <t>Mobile Action Plan</t>
   </si>
@@ -462,11 +462,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1004,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -1022,30 +1022,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="1"/>
@@ -1177,7 +1177,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="6"/>
@@ -1193,7 +1193,9 @@
       <c r="G11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
       <c r="B12" s="5" t="s">
@@ -1212,7 +1214,9 @@
       <c r="G12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
       <c r="B13" s="5" t="s">

</xml_diff>

<commit_message>
Slides 8 and 9 added
</commit_message>
<xml_diff>
--- a/MAP.xlsx
+++ b/MAP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
   <si>
     <t>Mobile Action Plan</t>
   </si>
@@ -1004,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -1235,7 +1235,9 @@
       <c r="G13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
       <c r="B14" s="5" t="s">
@@ -1254,7 +1256,9 @@
       <c r="G14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
       <c r="B15" s="5"/>
@@ -1544,7 +1548,9 @@
       <c r="G34" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H34" s="6"/>
+      <c r="H34" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="35" spans="2:8" ht="15" customHeight="1">
       <c r="B35" s="5"/>

</xml_diff>

<commit_message>
Added Mastery Slides 13, 14 and 15
</commit_message>
<xml_diff>
--- a/MAP.xlsx
+++ b/MAP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="103">
   <si>
     <t>Mobile Action Plan</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>Slides Folder</t>
+  </si>
+  <si>
+    <t>Video</t>
   </si>
 </sst>
 </file>
@@ -1004,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -1326,7 +1329,9 @@
       <c r="G18" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="15" customHeight="1">
       <c r="B19" s="5"/>
@@ -1341,7 +1346,9 @@
       <c r="G19" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="20" spans="2:8" ht="15" customHeight="1">
       <c r="B20" s="5"/>
@@ -1356,7 +1363,9 @@
       <c r="G20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="6"/>
+      <c r="H20" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1">
       <c r="B21" s="5"/>
@@ -1483,7 +1492,9 @@
       <c r="G29" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H29" s="6"/>
+      <c r="H29" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="30" spans="2:8" ht="15" customHeight="1">
       <c r="B30" s="5"/>
@@ -1496,7 +1507,9 @@
       <c r="G30" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="6"/>
+      <c r="H30" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="31" spans="2:8" ht="15" customHeight="1">
       <c r="B31" s="5"/>
@@ -1509,7 +1522,9 @@
       <c r="G31" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="H31" s="6"/>
+      <c r="H31" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1">
       <c r="B32" s="5"/>
@@ -1549,7 +1564,7 @@
         <v>88</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Added Some Code, signed app, icon and Slides 16, ,17 ,18 and 19
</commit_message>
<xml_diff>
--- a/MAP.xlsx
+++ b/MAP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="103">
   <si>
     <t>Mobile Action Plan</t>
   </si>
@@ -322,14 +322,14 @@
     <t>Slides Folder</t>
   </si>
   <si>
-    <t>Video</t>
+    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,6 +349,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -451,7 +459,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -470,6 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1007,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -1312,7 +1321,9 @@
       <c r="G17" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="15" customHeight="1">
       <c r="B18" s="5"/>
@@ -1382,7 +1393,9 @@
       <c r="G21" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="6"/>
+      <c r="H21" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="22" spans="2:8" ht="15" customHeight="1">
       <c r="B22" s="5"/>
@@ -1397,7 +1410,9 @@
       <c r="G22" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H22" s="6"/>
+      <c r="H22" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="23" spans="2:8" ht="15" customHeight="1">
       <c r="B23" s="5"/>
@@ -1412,7 +1427,9 @@
       <c r="G23" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H23" s="6"/>
+      <c r="H23" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="24" spans="2:8" ht="15" customHeight="1">
       <c r="B24" s="5"/>
@@ -1427,7 +1444,9 @@
       <c r="G24" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="H24" s="6"/>
+      <c r="H24" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="25" spans="2:8" ht="15" customHeight="1">
       <c r="B25" s="5"/>
@@ -1440,7 +1459,9 @@
       <c r="G25" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H25" s="6"/>
+      <c r="H25" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="26" spans="2:8" ht="15" customHeight="1">
       <c r="B26" s="5"/>
@@ -1453,7 +1474,9 @@
       <c r="G26" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H26" s="6"/>
+      <c r="H26" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="27" spans="2:8" ht="15" customHeight="1">
       <c r="B27" s="5"/>
@@ -1479,7 +1502,9 @@
       <c r="G28" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="6"/>
+      <c r="H28" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="29" spans="2:8" ht="15" customHeight="1">
       <c r="B29" s="5"/>
@@ -1493,7 +1518,7 @@
         <v>78</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="15" customHeight="1">
@@ -1508,7 +1533,7 @@
         <v>80</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="15" customHeight="1">
@@ -1523,7 +1548,7 @@
         <v>82</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1">
@@ -1550,7 +1575,9 @@
       <c r="G33" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H33" s="6"/>
+      <c r="H33" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="34" spans="2:8" ht="15" customHeight="1">
       <c r="B34" s="5"/>
@@ -1564,7 +1591,7 @@
         <v>88</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="15" customHeight="1">
@@ -1578,7 +1605,9 @@
       <c r="G35" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="H35" s="6"/>
+      <c r="H35" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="36" spans="2:8" ht="15" customHeight="1">
       <c r="B36" s="5"/>

</xml_diff>

<commit_message>
Created MyApp (final project) wich contains the structure of the main app
</commit_message>
<xml_diff>
--- a/MAP.xlsx
+++ b/MAP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
   <si>
     <t>Mobile Action Plan</t>
   </si>
@@ -475,10 +475,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -1034,27 +1034,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
@@ -1444,7 +1444,7 @@
       <c r="G24" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="13" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1605,9 +1605,7 @@
       <c r="G35" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>100</v>
-      </c>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" spans="2:8" ht="15" customHeight="1">
       <c r="B36" s="5"/>

</xml_diff>